<commit_message>
Added fallback logback.xml. Fixed FileUtils bug not working with spaces
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="templateResultSheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -389,7 +389,7 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -626,7 +626,7 @@
   </sheetPr>
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Y2" activeCellId="0" sqref="Y2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added local plot for datasets and groups. Added dark data plot
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
   <si>
     <t xml:space="preserve">Cell</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">#UIChart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#UIChartDark</t>
   </si>
   <si>
     <t xml:space="preserve">#groupname</t>
@@ -390,7 +393,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -505,6 +508,9 @@
       </c>
       <c r="D10" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -544,25 +550,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
@@ -582,22 +588,22 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>18</v>
@@ -638,174 +644,174 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug that resulted in falsly written ISC and JSC in result files
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t xml:space="preserve">Cell</t>
   </si>
@@ -30,19 +30,16 @@
     <t xml:space="preserve">VOC[V]</t>
   </si>
   <si>
-    <t xml:space="preserve">Jsc[V/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rs[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RsDark[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rp[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RpDark[ohm/cm^2]</t>
+    <t xml:space="preserve">Jsc[A/cm^2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RsDark[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rp[ohm]</t>
   </si>
   <si>
     <t xml:space="preserve">MP[W/cm^2]</t>
@@ -60,7 +57,7 @@
     <t xml:space="preserve">#voc</t>
   </si>
   <si>
-    <t xml:space="preserve">#isc</t>
+    <t xml:space="preserve">#jsc</t>
   </si>
   <si>
     <t xml:space="preserve">#rs</t>
@@ -117,37 +114,13 @@
     <t xml:space="preserve">#groupname</t>
   </si>
   <si>
-    <t xml:space="preserve">VOC [V]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JSC[A/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RP[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RP_Dark[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_Dark[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#jsc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rp#divideByArea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rpDark#divideByArea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rs#divideByArea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rsDark#divideByArea</t>
+    <t xml:space="preserve">Voc[V]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs_Dark[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rp_Dark[ohm]</t>
   </si>
   <si>
     <t xml:space="preserve">#mp#divideByArea</t>
@@ -171,37 +144,40 @@
     <t xml:space="preserve">JSC_MAX[V/cm^2]</t>
   </si>
   <si>
-    <t xml:space="preserve">RP_STD[ohm/cm^2[</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RP_MAX[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RP_DARK[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RP_DARK_STD[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RP_DARK_MAX[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS[ohm/cm^2[</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_STD[ohm/cm^2[</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_MAX[ohm/cm^2[</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_DARK[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_DARK_STD[ohm/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_DARK_MAX[ohm/cm^2]</t>
+    <t xml:space="preserve">RP[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP_STD[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP_MAX[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP_DARK[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP_DARK_STD[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP_DARK_MAX[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS_STD[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS_MAX[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS_DARK[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS_DARK_STD[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS_DARK_MAX[ohm]</t>
   </si>
   <si>
     <t xml:space="preserve">MP_STD[W/cm^2]</t>
@@ -240,28 +216,28 @@
     <t xml:space="preserve">#jsc#max</t>
   </si>
   <si>
-    <t xml:space="preserve">#rp#divideByArea#std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rp#divideByArea#max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rpDark#divideByArea#std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rpDark#divideByArea#max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rs#divideByArea#std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rs#divideByArea#max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rsDark#divideByArea#std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#rsDark#divideByArea#max</t>
+    <t xml:space="preserve">#rp#std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#rp#max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#rpDark#std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#rpDark#max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#rs#std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#rs#max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#rsDark#std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#rsDark#max</t>
   </si>
   <si>
     <t xml:space="preserve">#mp#divideByArea#std</t>
@@ -393,7 +369,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -428,48 +404,48 @@
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,40 +453,40 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="I10" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -532,7 +508,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -550,66 +526,66 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -633,7 +609,7 @@
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y2" activeCellId="0" sqref="Y2"/>
+      <selection pane="topLeft" activeCell="P5" activeCellId="0" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -644,174 +620,174 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="O1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="P1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="T1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="V1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="W1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Z1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="AB1" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA1" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="F2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="T2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="W2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="0" t="s">
+      <c r="Z2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA2" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="AB2" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adde new chart features
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t xml:space="preserve">Cell</t>
   </si>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">#rpDark</t>
   </si>
   <si>
-    <t xml:space="preserve">#mp</t>
+    <t xml:space="preserve">#mp#divideByArea</t>
   </si>
   <si>
     <t xml:space="preserve">#eff</t>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t xml:space="preserve">Rp_Dark[ohm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#mp#divideByArea</t>
   </si>
   <si>
     <t xml:space="preserve">Group</t>
@@ -369,7 +366,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -579,7 +576,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>17</v>
@@ -620,88 +617,88 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="X1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AB1" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,82 +709,82 @@
         <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>15</v>
       </c>
       <c r="L2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="O2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="Q2" s="0" t="s">
         <v>13</v>
       </c>
       <c r="R2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="T2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="W2" s="0" t="s">
         <v>17</v>
       </c>
       <c r="X2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y2" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="AA2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB2" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished UI Method to evaluate labview data
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="templateResultSheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -42,7 +42,7 @@
     <t xml:space="preserve">Rp[ohm]</t>
   </si>
   <si>
-    <t xml:space="preserve">MP[W/cm^2]</t>
+    <t xml:space="preserve">Pmpp[W/cm^2]</t>
   </si>
   <si>
     <t xml:space="preserve">Efficiency[%]</t>
@@ -177,10 +177,10 @@
     <t xml:space="preserve">RS_DARK_MAX[ohm]</t>
   </si>
   <si>
-    <t xml:space="preserve">MP_STD[W/cm^2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MP_MAX[W/cm^2]</t>
+    <t xml:space="preserve">Pmpp_STD[W/cm^2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pmpp_MAX[W/cm^2]</t>
   </si>
   <si>
     <t xml:space="preserve">EFF[%]</t>
@@ -365,8 +365,8 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -605,8 +605,8 @@
   </sheetPr>
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P5" activeCellId="0" sqref="P5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Imroved Excel Export, added FileDialogWithLastOpen class
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t xml:space="preserve">Cell</t>
   </si>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">Rp[ohm]</t>
   </si>
   <si>
+    <t xml:space="preserve">RpDark[ohm]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pmpp[W/cm^2]</t>
   </si>
   <si>
@@ -97,6 +100,9 @@
   </si>
   <si>
     <t xml:space="preserve">#powerInput</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#UIChartLightDark</t>
   </si>
   <si>
     <t xml:space="preserve">Voltage[V]</t>
@@ -369,10 +375,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,54 +415,54 @@
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,40 +470,45 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="0" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -519,7 +530,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="D33:H33 K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -533,16 +544,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -551,60 +562,60 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="1"/>
     </row>
@@ -627,7 +638,7 @@
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
+      <selection pane="topLeft" activeCell="U5" activeCellId="1" sqref="D33:H33 U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -638,174 +649,174 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="R2" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Vmpp and Impp to data output (FXTable and Excel)
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="templateResultSheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
   <si>
     <t xml:space="preserve">Cell</t>
   </si>
@@ -48,6 +48,12 @@
     <t xml:space="preserve">Pmpp[W/cm^2]</t>
   </si>
   <si>
+    <t xml:space="preserve">Vmpp[V]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impp[A]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Efficiency[%]</t>
   </si>
   <si>
@@ -81,6 +87,12 @@
     <t xml:space="preserve">#mp#divideByArea</t>
   </si>
   <si>
+    <t xml:space="preserve">#vmpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#impp</t>
+  </si>
+  <si>
     <t xml:space="preserve">#eff</t>
   </si>
   <si>
@@ -195,6 +207,18 @@
     <t xml:space="preserve">Pmpp_MAX[W/cm^2]</t>
   </si>
   <si>
+    <t xml:space="preserve">Vmpp_STD[V]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vmpp_MAX[V]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impp_STD[A]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impp_MAX[V]</t>
+  </si>
+  <si>
     <t xml:space="preserve">EFF[%]</t>
   </si>
   <si>
@@ -253,6 +277,18 @@
   </si>
   <si>
     <t xml:space="preserve">#mp#divideByArea#max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#vmpp#std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#vmpp#max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#impp#std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#impp#max</t>
   </si>
   <si>
     <t xml:space="preserve">#eff#std</t>
@@ -375,10 +411,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33:H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,40 +465,52 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,45 +518,45 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -527,10 +575,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="D33:H33 K3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,18 +590,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -562,13 +612,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
@@ -582,42 +632,53 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -635,10 +696,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U5" activeCellId="1" sqref="D33:H33 U5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -649,174 +710,210 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="O2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="R2" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DarkData to Cell Result export, Added Suffix to CellGroups
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="templateResultSheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="102">
   <si>
     <t xml:space="preserve">Cell</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve">Voc Per Cell[V]</t>
   </si>
   <si>
+    <t xml:space="preserve">Cells</t>
+  </si>
+  <si>
     <t xml:space="preserve">#name</t>
   </si>
   <si>
@@ -102,6 +105,9 @@
     <t xml:space="preserve">#voc#divideByCells</t>
   </si>
   <si>
+    <t xml:space="preserve">#cells</t>
+  </si>
+  <si>
     <t xml:space="preserve">Area[cm^2]</t>
   </si>
   <si>
@@ -123,12 +129,30 @@
     <t xml:space="preserve">Current[A]</t>
   </si>
   <si>
+    <t xml:space="preserve">Dark Voltage[V]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DarkCurrent[A]</t>
+  </si>
+  <si>
     <t xml:space="preserve">#voltageData</t>
   </si>
   <si>
     <t xml:space="preserve">#currentData</t>
   </si>
   <si>
+    <t xml:space="preserve">#darkVoltageData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#darkCurrentData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark Data</t>
+  </si>
+  <si>
     <t xml:space="preserve">#UIChart</t>
   </si>
   <si>
@@ -235,6 +259,9 @@
   </si>
   <si>
     <t xml:space="preserve">FF_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELLS_MEAN</t>
   </si>
   <si>
     <t xml:space="preserve">#voc#std</t>
@@ -411,24 +438,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="14.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,46 +490,52 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,45 +543,65 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>36</v>
+      <c r="F33" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -575,7 +620,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -584,26 +629,16 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="0" width="14.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -612,13 +647,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
@@ -638,46 +673,52 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -696,9 +737,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -710,210 +751,216 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="W1" s="0" t="s">
         <v>8</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="Z1" s="0" t="s">
         <v>9</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="R2" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increased Version -> Made RS and RS Dark Min to be the best value
</commit_message>
<xml_diff>
--- a/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
+++ b/features/at.sunplugged.celldatabaseV2.feature/rootfiles/excelTemplate/template.xlsx
@@ -213,7 +213,7 @@
     <t xml:space="preserve">RS_STD[ohm]</t>
   </si>
   <si>
-    <t xml:space="preserve">RS_MAX[ohm]</t>
+    <t xml:space="preserve">RS_MIN[ohm]</t>
   </si>
   <si>
     <t xml:space="preserve">RS_DARK[ohm]</t>
@@ -222,7 +222,7 @@
     <t xml:space="preserve">RS_DARK_STD[ohm]</t>
   </si>
   <si>
-    <t xml:space="preserve">RS_DARK_MAX[ohm]</t>
+    <t xml:space="preserve">RS_DARK_MIN[ohm]</t>
   </si>
   <si>
     <t xml:space="preserve">Pmpp_STD[W/cm^2]</t>
@@ -291,13 +291,13 @@
     <t xml:space="preserve">#rs#std</t>
   </si>
   <si>
-    <t xml:space="preserve">#rs#max</t>
+    <t xml:space="preserve">#rs#min</t>
   </si>
   <si>
     <t xml:space="preserve">#rsDark#std</t>
   </si>
   <si>
-    <t xml:space="preserve">#rsDark#max</t>
+    <t xml:space="preserve">#rsDark#min</t>
   </si>
   <si>
     <t xml:space="preserve">#mp#divideByArea#std</t>

</xml_diff>